<commit_message>
Modifiche prima dell'implementazione della logica principale.
</commit_message>
<xml_diff>
--- a/ESP_FATT.xlsx
+++ b/ESP_FATT.xlsx
@@ -464,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J101"/>
+  <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -482,6 +482,7 @@
     <col customWidth="true" min="8" max="8" width="13.8359375"/>
     <col customWidth="true" min="9" max="9" width="13.8359375"/>
     <col customWidth="true" min="10" max="10" width="13.8359375"/>
+    <col customWidth="true" min="11" max="11" width="13.8359375"/>
   </cols>
   <sheetData>
     <row outlineLevel="0" r="1">
@@ -535,6 +536,11 @@
           <t>dd_prodest</t>
         </is>
       </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>tm_vettor</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="2">
       <c r="A2" s="4">
@@ -583,6 +589,11 @@
           <t/>
         </is>
       </c>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="3">
       <c r="A3" s="4">
@@ -631,6 +642,11 @@
           <t/>
         </is>
       </c>
+      <c r="K3" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="4">
       <c r="A4" s="4">
@@ -679,6 +695,11 @@
           <t/>
         </is>
       </c>
+      <c r="K4" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="5">
       <c r="A5" s="4">
@@ -727,6 +748,11 @@
           <t/>
         </is>
       </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="4">
@@ -775,6 +801,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="4">
@@ -823,6 +854,11 @@
           <t/>
         </is>
       </c>
+      <c r="K7" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="4">
@@ -871,6 +907,11 @@
           <t/>
         </is>
       </c>
+      <c r="K8" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="4">
@@ -919,6 +960,11 @@
           <t/>
         </is>
       </c>
+      <c r="K9" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="4">
@@ -967,6 +1013,11 @@
           <t/>
         </is>
       </c>
+      <c r="K10" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="4">
@@ -1015,6 +1066,11 @@
           <t/>
         </is>
       </c>
+      <c r="K11" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="4">
@@ -1063,6 +1119,11 @@
           <t/>
         </is>
       </c>
+      <c r="K12" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="4">
@@ -1111,6 +1172,11 @@
           <t/>
         </is>
       </c>
+      <c r="K13" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="4">
@@ -1159,6 +1225,11 @@
           <t/>
         </is>
       </c>
+      <c r="K14" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="15">
       <c r="A15" s="4">
@@ -1207,6 +1278,11 @@
           <t/>
         </is>
       </c>
+      <c r="K15" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="16">
       <c r="A16" s="4">
@@ -1255,6 +1331,11 @@
           <t/>
         </is>
       </c>
+      <c r="K16" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="17">
       <c r="A17" s="4">
@@ -1303,6 +1384,11 @@
           <t/>
         </is>
       </c>
+      <c r="K17" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="18">
       <c r="A18" s="4">
@@ -1351,6 +1437,11 @@
           <t/>
         </is>
       </c>
+      <c r="K18" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="19">
       <c r="A19" s="4">
@@ -1399,6 +1490,11 @@
           <t/>
         </is>
       </c>
+      <c r="K19" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="20">
       <c r="A20" s="4">
@@ -1447,6 +1543,11 @@
           <t/>
         </is>
       </c>
+      <c r="K20" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="21">
       <c r="A21" s="4">
@@ -1495,6 +1596,11 @@
           <t/>
         </is>
       </c>
+      <c r="K21" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="22">
       <c r="A22" s="4">
@@ -1543,6 +1649,11 @@
           <t/>
         </is>
       </c>
+      <c r="K22" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="23">
       <c r="A23" s="4">
@@ -1591,6 +1702,11 @@
           <t/>
         </is>
       </c>
+      <c r="K23" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="24">
       <c r="A24" s="4">
@@ -1639,6 +1755,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="K24" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="25">
       <c r="A25" s="4">
@@ -1687,6 +1808,11 @@
           <t/>
         </is>
       </c>
+      <c r="K25" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="26">
       <c r="A26" s="4">
@@ -1735,6 +1861,11 @@
           <t/>
         </is>
       </c>
+      <c r="K26" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="27">
       <c r="A27" s="4">
@@ -1783,6 +1914,11 @@
           <t/>
         </is>
       </c>
+      <c r="K27" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="28">
       <c r="A28" s="4">
@@ -1831,6 +1967,11 @@
           <t/>
         </is>
       </c>
+      <c r="K28" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="29">
       <c r="A29" s="4">
@@ -1879,6 +2020,11 @@
           <t/>
         </is>
       </c>
+      <c r="K29" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="30">
       <c r="A30" s="4">
@@ -1927,6 +2073,11 @@
           <t/>
         </is>
       </c>
+      <c r="K30" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="31">
       <c r="A31" s="4">
@@ -1975,6 +2126,11 @@
           <t/>
         </is>
       </c>
+      <c r="K31" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="32">
       <c r="A32" s="4">
@@ -2023,6 +2179,11 @@
           <t/>
         </is>
       </c>
+      <c r="K32" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="33">
       <c r="A33" s="4">
@@ -2071,6 +2232,11 @@
           <t/>
         </is>
       </c>
+      <c r="K33" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="4">
@@ -2119,6 +2285,11 @@
           <t/>
         </is>
       </c>
+      <c r="K34" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="4">
@@ -2167,6 +2338,11 @@
           <t/>
         </is>
       </c>
+      <c r="K35" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="4">
@@ -2215,6 +2391,11 @@
           <t/>
         </is>
       </c>
+      <c r="K36" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="4">
@@ -2263,6 +2444,11 @@
           <t/>
         </is>
       </c>
+      <c r="K37" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="4">
@@ -2311,6 +2497,11 @@
           <t/>
         </is>
       </c>
+      <c r="K38" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="4">
@@ -2359,6 +2550,11 @@
           <t>MS</t>
         </is>
       </c>
+      <c r="K39" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="4">
@@ -2407,6 +2603,11 @@
           <t/>
         </is>
       </c>
+      <c r="K40" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="41">
       <c r="A41" s="4">
@@ -2455,6 +2656,11 @@
           <t/>
         </is>
       </c>
+      <c r="K41" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="42">
       <c r="A42" s="4">
@@ -2503,6 +2709,11 @@
           <t/>
         </is>
       </c>
+      <c r="K42" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="43">
       <c r="A43" s="4">
@@ -2551,6 +2762,11 @@
           <t>MS</t>
         </is>
       </c>
+      <c r="K43" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="44">
       <c r="A44" s="4">
@@ -2599,6 +2815,11 @@
           <t/>
         </is>
       </c>
+      <c r="K44" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="45">
       <c r="A45" s="4">
@@ -2647,6 +2868,11 @@
           <t/>
         </is>
       </c>
+      <c r="K45" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="46">
       <c r="A46" s="4">
@@ -2695,6 +2921,11 @@
           <t/>
         </is>
       </c>
+      <c r="K46" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="47">
       <c r="A47" s="4">
@@ -2743,6 +2974,11 @@
           <t/>
         </is>
       </c>
+      <c r="K47" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="48">
       <c r="A48" s="4">
@@ -2791,6 +3027,11 @@
           <t/>
         </is>
       </c>
+      <c r="K48" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="49">
       <c r="A49" s="4">
@@ -2839,6 +3080,11 @@
           <t/>
         </is>
       </c>
+      <c r="K49" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="50">
       <c r="A50" s="4">
@@ -2887,6 +3133,11 @@
           <t/>
         </is>
       </c>
+      <c r="K50" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="51">
       <c r="A51" s="4">
@@ -2935,6 +3186,11 @@
           <t/>
         </is>
       </c>
+      <c r="K51" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="52">
       <c r="A52" s="4">
@@ -2983,6 +3239,11 @@
           <t/>
         </is>
       </c>
+      <c r="K52" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="53">
       <c r="A53" s="4">
@@ -3031,6 +3292,11 @@
           <t>SP</t>
         </is>
       </c>
+      <c r="K53" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="54">
       <c r="A54" s="4">
@@ -3079,6 +3345,11 @@
           <t/>
         </is>
       </c>
+      <c r="K54" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="55">
       <c r="A55" s="4">
@@ -3127,6 +3398,11 @@
           <t/>
         </is>
       </c>
+      <c r="K55" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="56">
       <c r="A56" s="4">
@@ -3175,6 +3451,11 @@
           <t/>
         </is>
       </c>
+      <c r="K56" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="57">
       <c r="A57" s="4">
@@ -3223,6 +3504,11 @@
           <t/>
         </is>
       </c>
+      <c r="K57" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="58">
       <c r="A58" s="4">
@@ -3271,6 +3557,11 @@
           <t/>
         </is>
       </c>
+      <c r="K58" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="59">
       <c r="A59" s="4">
@@ -3319,6 +3610,11 @@
           <t/>
         </is>
       </c>
+      <c r="K59" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="60">
       <c r="A60" s="4">
@@ -3367,6 +3663,11 @@
           <t/>
         </is>
       </c>
+      <c r="K60" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="61">
       <c r="A61" s="4">
@@ -3415,6 +3716,11 @@
           <t/>
         </is>
       </c>
+      <c r="K61" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="62">
       <c r="A62" s="4">
@@ -3463,6 +3769,11 @@
           <t/>
         </is>
       </c>
+      <c r="K62" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="63">
       <c r="A63" s="4">
@@ -3511,6 +3822,11 @@
           <t/>
         </is>
       </c>
+      <c r="K63" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="64">
       <c r="A64" s="4">
@@ -3559,6 +3875,11 @@
           <t/>
         </is>
       </c>
+      <c r="K64" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="65">
       <c r="A65" s="4">
@@ -3607,6 +3928,11 @@
           <t/>
         </is>
       </c>
+      <c r="K65" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="66">
       <c r="A66" s="4">
@@ -3655,6 +3981,11 @@
           <t/>
         </is>
       </c>
+      <c r="K66" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="67">
       <c r="A67" s="4">
@@ -3703,6 +4034,11 @@
           <t/>
         </is>
       </c>
+      <c r="K67" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="68">
       <c r="A68" s="4">
@@ -3751,6 +4087,11 @@
           <t/>
         </is>
       </c>
+      <c r="K68" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="69">
       <c r="A69" s="4">
@@ -3799,6 +4140,11 @@
           <t/>
         </is>
       </c>
+      <c r="K69" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="70">
       <c r="A70" s="4">
@@ -3847,6 +4193,11 @@
           <t/>
         </is>
       </c>
+      <c r="K70" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="71">
       <c r="A71" s="4">
@@ -3895,6 +4246,11 @@
           <t/>
         </is>
       </c>
+      <c r="K71" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="72">
       <c r="A72" s="4">
@@ -3943,6 +4299,11 @@
           <t/>
         </is>
       </c>
+      <c r="K72" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="73">
       <c r="A73" s="4">
@@ -3991,6 +4352,11 @@
           <t/>
         </is>
       </c>
+      <c r="K73" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="74">
       <c r="A74" s="4">
@@ -4039,6 +4405,11 @@
           <t/>
         </is>
       </c>
+      <c r="K74" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="75">
       <c r="A75" s="4">
@@ -4087,6 +4458,11 @@
           <t/>
         </is>
       </c>
+      <c r="K75" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="76">
       <c r="A76" s="4">
@@ -4135,6 +4511,11 @@
           <t/>
         </is>
       </c>
+      <c r="K76" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="77">
       <c r="A77" s="4">
@@ -4183,6 +4564,11 @@
           <t/>
         </is>
       </c>
+      <c r="K77" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="78">
       <c r="A78" s="4">
@@ -4231,6 +4617,11 @@
           <t/>
         </is>
       </c>
+      <c r="K78" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="79">
       <c r="A79" s="4">
@@ -4279,6 +4670,11 @@
           <t/>
         </is>
       </c>
+      <c r="K79" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="80">
       <c r="A80" s="4">
@@ -4327,6 +4723,11 @@
           <t/>
         </is>
       </c>
+      <c r="K80" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="81">
       <c r="A81" s="4">
@@ -4375,6 +4776,11 @@
           <t>MS</t>
         </is>
       </c>
+      <c r="K81" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="82">
       <c r="A82" s="4">
@@ -4423,6 +4829,11 @@
           <t/>
         </is>
       </c>
+      <c r="K82" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="83">
       <c r="A83" s="4">
@@ -4471,6 +4882,11 @@
           <t/>
         </is>
       </c>
+      <c r="K83" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="84">
       <c r="A84" s="4">
@@ -4519,6 +4935,11 @@
           <t/>
         </is>
       </c>
+      <c r="K84" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="85">
       <c r="A85" s="4">
@@ -4567,6 +4988,11 @@
           <t/>
         </is>
       </c>
+      <c r="K85" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="86">
       <c r="A86" s="4">
@@ -4615,6 +5041,11 @@
           <t/>
         </is>
       </c>
+      <c r="K86" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="87">
       <c r="A87" s="4">
@@ -4663,6 +5094,11 @@
           <t/>
         </is>
       </c>
+      <c r="K87" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="88">
       <c r="A88" s="4">
@@ -4711,6 +5147,11 @@
           <t/>
         </is>
       </c>
+      <c r="K88" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="89">
       <c r="A89" s="4">
@@ -4759,6 +5200,11 @@
           <t/>
         </is>
       </c>
+      <c r="K89" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="90">
       <c r="A90" s="4">
@@ -4807,6 +5253,11 @@
           <t>MS</t>
         </is>
       </c>
+      <c r="K90" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="91">
       <c r="A91" s="4">
@@ -4855,6 +5306,11 @@
           <t/>
         </is>
       </c>
+      <c r="K91" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="92">
       <c r="A92" s="4">
@@ -4903,6 +5359,11 @@
           <t/>
         </is>
       </c>
+      <c r="K92" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="93">
       <c r="A93" s="4">
@@ -4951,6 +5412,11 @@
           <t/>
         </is>
       </c>
+      <c r="K93" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="94">
       <c r="A94" s="4">
@@ -4999,6 +5465,11 @@
           <t/>
         </is>
       </c>
+      <c r="K94" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="95">
       <c r="A95" s="4">
@@ -5047,6 +5518,11 @@
           <t/>
         </is>
       </c>
+      <c r="K95" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="96">
       <c r="A96" s="4">
@@ -5095,6 +5571,11 @@
           <t/>
         </is>
       </c>
+      <c r="K96" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="97">
       <c r="A97" s="4">
@@ -5143,6 +5624,11 @@
           <t/>
         </is>
       </c>
+      <c r="K97" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="98">
       <c r="A98" s="4">
@@ -5191,6 +5677,11 @@
           <t/>
         </is>
       </c>
+      <c r="K98" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="99">
       <c r="A99" s="4">
@@ -5239,6 +5730,11 @@
           <t/>
         </is>
       </c>
+      <c r="K99" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="100">
       <c r="A100" s="4">
@@ -5287,6 +5783,11 @@
           <t/>
         </is>
       </c>
+      <c r="K100" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row outlineLevel="0" r="101">
       <c r="A101" s="4">
@@ -5333,6 +5834,11 @@
       <c r="J101" s="5" t="inlineStr">
         <is>
           <t/>
+        </is>
+      </c>
+      <c r="K101" s="5" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>